<commit_message>
Mean & conditional mean imputation
</commit_message>
<xml_diff>
--- a/Output/Models/Mean_Imputation_Validation.xlsx
+++ b/Output/Models/Mean_Imputation_Validation.xlsx
@@ -434,25 +434,25 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>0.2286999769788207</v>
+        <v>0.177040614553816</v>
       </c>
       <c r="F2">
-        <v>0.04677249111707563</v>
+        <v>0.03271345881050904</v>
       </c>
       <c r="G2">
-        <v>0.3270247615229064</v>
+        <v>0.4119776363568582</v>
       </c>
       <c r="H2">
-        <v>0.00634373099659391</v>
+        <v>0.008006391738267952</v>
       </c>
       <c r="I2">
-        <v>0.9795158442212608</v>
+        <v>0.9842737936058645</v>
       </c>
       <c r="J2">
-        <v>0.9227833995275387</v>
+        <v>0.9399032630736774</v>
       </c>
       <c r="K2">
-        <v>0.922842810676723</v>
+        <v>0.9400261706758157</v>
       </c>
     </row>
     <row r="3">
@@ -475,25 +475,25 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>0.2316170719182071</v>
+        <v>0.2504929342755191</v>
       </c>
       <c r="F3">
-        <v>0.06498499501875343</v>
+        <v>0.06579994006005384</v>
       </c>
       <c r="G3">
-        <v>0.3942917213053653</v>
+        <v>0.9075282800135882</v>
       </c>
       <c r="H3">
-        <v>0.007648597012951301</v>
+        <v>0.01763694502351926</v>
       </c>
       <c r="I3">
-        <v>0.9789609104299575</v>
+        <v>0.9670114716162004</v>
       </c>
       <c r="J3">
-        <v>0.9208010233966855</v>
+        <v>0.8796915767461381</v>
       </c>
       <c r="K3">
-        <v>0.9208873892353878</v>
+        <v>0.8802879961950569</v>
       </c>
     </row>
     <row r="4">
@@ -516,25 +516,25 @@
         <v>20</v>
       </c>
       <c r="E4">
-        <v>0.4335231978517848</v>
+        <v>0.350764879548896</v>
       </c>
       <c r="F4">
-        <v>0.1675796358081236</v>
+        <v>0.1287472743760802</v>
       </c>
       <c r="G4">
-        <v>3.49184181192812</v>
+        <v>1.953999776834536</v>
       </c>
       <c r="H4">
-        <v>0.06773586512035258</v>
+        <v>0.03797411871229358</v>
       </c>
       <c r="I4">
-        <v>0.9143288447556132</v>
+        <v>0.9290822933606959</v>
       </c>
       <c r="J4">
-        <v>0.7225382514483669</v>
+        <v>0.7640949266995968</v>
       </c>
       <c r="K4">
-        <v>0.7293117930061743</v>
+        <v>0.7668598334082359</v>
       </c>
     </row>
     <row r="5">
@@ -557,25 +557,25 @@
         <v>40</v>
       </c>
       <c r="E5">
-        <v>0.5594106614387977</v>
+        <v>0.5026378515062118</v>
       </c>
       <c r="F5">
-        <v>0.2975230994342121</v>
+        <v>0.2578747337779352</v>
       </c>
       <c r="G5">
-        <v>6.187050324056158</v>
+        <v>4.555505770754011</v>
       </c>
       <c r="H5">
-        <v>0.1200183825084825</v>
+        <v>0.08853190209335432</v>
       </c>
       <c r="I5">
-        <v>0.836594697239901</v>
+        <v>0.8213773232463539</v>
       </c>
       <c r="J5">
-        <v>0.538002193245576</v>
+        <v>0.5155873726728482</v>
       </c>
       <c r="K5">
-        <v>0.5592676137383528</v>
+        <v>0.5306154930423113</v>
       </c>
     </row>
     <row r="6">
@@ -598,25 +598,25 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>0.1786183798699327</v>
+        <v>0.1660203616698156</v>
       </c>
       <c r="F6">
-        <v>0.03297992366308788</v>
+        <v>0.0310521315129072</v>
       </c>
       <c r="G6">
-        <v>0.8204284337711117</v>
+        <v>0.05602688982520403</v>
       </c>
       <c r="H6">
-        <v>0.0159149333572291</v>
+        <v>-0.001088829072820848</v>
       </c>
       <c r="I6">
-        <v>0.9878053635079638</v>
+        <v>0.9862432539284421</v>
       </c>
       <c r="J6">
-        <v>0.9528989349585066</v>
+        <v>0.9471520937351563</v>
       </c>
       <c r="K6">
-        <v>0.9532728630427479</v>
+        <v>0.9471543668663025</v>
       </c>
     </row>
     <row r="7">
@@ -639,25 +639,25 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>0.2261844660266443</v>
+        <v>0.2274589130094877</v>
       </c>
       <c r="F7">
-        <v>0.06148183945927491</v>
+        <v>0.05977118312009332</v>
       </c>
       <c r="G7">
-        <v>0.5886223497368951</v>
+        <v>0.05155052184960606</v>
       </c>
       <c r="H7">
-        <v>-0.01141828474371452</v>
+        <v>-0.001001835138164088</v>
       </c>
       <c r="I7">
-        <v>0.9800012516173278</v>
+        <v>0.9732083559213293</v>
       </c>
       <c r="J7">
-        <v>0.9244726954451035</v>
+        <v>0.9008001549960689</v>
       </c>
       <c r="K7">
-        <v>0.9246651730357898</v>
+        <v>0.9008020794060287</v>
       </c>
     </row>
     <row r="8">
@@ -680,25 +680,25 @@
         <v>20</v>
       </c>
       <c r="E8">
-        <v>0.3640996830836913</v>
+        <v>0.3173328993539681</v>
       </c>
       <c r="F8">
-        <v>0.1443015511293844</v>
+        <v>0.1176754147957396</v>
       </c>
       <c r="G8">
-        <v>1.321745111977015</v>
+        <v>0.07103903785795875</v>
       </c>
       <c r="H8">
-        <v>-0.02563963474019004</v>
+        <v>-0.001380575826469851</v>
       </c>
       <c r="I8">
-        <v>0.9429259253641343</v>
+        <v>0.9435673203049786</v>
       </c>
       <c r="J8">
-        <v>0.8042872868474049</v>
+        <v>0.8069208962233845</v>
       </c>
       <c r="K8">
-        <v>0.8052578015157281</v>
+        <v>0.8069245507035201</v>
       </c>
     </row>
     <row r="9">
@@ -721,25 +721,25 @@
         <v>40</v>
       </c>
       <c r="E9">
-        <v>0.5311378500815386</v>
+        <v>0.4572649771465216</v>
       </c>
       <c r="F9">
-        <v>0.288301770262534</v>
+        <v>0.2398180566095743</v>
       </c>
       <c r="G9">
-        <v>0.4883000656542348</v>
+        <v>0.2584969347059904</v>
       </c>
       <c r="H9">
-        <v>-0.009472200966386566</v>
+        <v>0.005023640944929605</v>
       </c>
       <c r="I9">
-        <v>0.8490635007165203</v>
+        <v>0.8569303371359109</v>
       </c>
       <c r="J9">
-        <v>0.5835211626408924</v>
+        <v>0.5990954796412684</v>
       </c>
       <c r="K9">
-        <v>0.5836536212660638</v>
+        <v>0.5991438681522158</v>
       </c>
     </row>
     <row r="10">
@@ -762,25 +762,25 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <v>0.1565791329328627</v>
+        <v>0.14841338187132</v>
       </c>
       <c r="F10">
-        <v>0.0312010526840897</v>
+        <v>0.02896461124791324</v>
       </c>
       <c r="G10">
-        <v>1.267505836581525</v>
+        <v>1.128162121046377</v>
       </c>
       <c r="H10">
-        <v>-0.02458748391541202</v>
+        <v>-0.02192475291923015</v>
       </c>
       <c r="I10">
-        <v>0.9907166379304227</v>
+        <v>0.989118351435694</v>
       </c>
       <c r="J10">
-        <v>0.9638051981554666</v>
+        <v>0.9577670714574064</v>
       </c>
       <c r="K10">
-        <v>0.9646976948439494</v>
+        <v>0.9586887394174771</v>
       </c>
     </row>
     <row r="11">
@@ -803,25 +803,25 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>0.2727563303141231</v>
+        <v>0.2090171111843771</v>
       </c>
       <c r="F11">
-        <v>0.07974735651236271</v>
+        <v>0.05791753302368297</v>
       </c>
       <c r="G11">
-        <v>3.784942445285886</v>
+        <v>2.262589300265958</v>
       </c>
       <c r="H11">
-        <v>-0.07342152502052111</v>
+        <v>-0.0439712612581022</v>
       </c>
       <c r="I11">
-        <v>0.9705748755841925</v>
+        <v>0.9778366781061348</v>
       </c>
       <c r="J11">
-        <v>0.8901681969358769</v>
+        <v>0.9162338110769621</v>
       </c>
       <c r="K11">
-        <v>0.8981265872955405</v>
+        <v>0.9199409846516621</v>
       </c>
     </row>
     <row r="12">
@@ -844,25 +844,25 @@
         <v>20</v>
       </c>
       <c r="E12">
-        <v>0.3566221408531747</v>
+        <v>0.3113067625788649</v>
       </c>
       <c r="F12">
-        <v>0.1436258255804584</v>
+        <v>0.1214975840605807</v>
       </c>
       <c r="G12">
-        <v>5.366658326655765</v>
+        <v>4.831866850497923</v>
       </c>
       <c r="H12">
-        <v>-0.1041041559556349</v>
+        <v>-0.09390271562878576</v>
       </c>
       <c r="I12">
-        <v>0.9473534984444224</v>
+        <v>0.9480491465028942</v>
       </c>
       <c r="J12">
-        <v>0.8122434738669492</v>
+        <v>0.8141843944919857</v>
       </c>
       <c r="K12">
-        <v>0.8282432744772088</v>
+        <v>0.8310911930815574</v>
       </c>
     </row>
     <row r="13">
@@ -885,25 +885,25 @@
         <v>40</v>
       </c>
       <c r="E13">
-        <v>0.6056800413230904</v>
+        <v>0.4932480576010425</v>
       </c>
       <c r="F13">
-        <v>0.3472441397591964</v>
+        <v>0.2756586299876386</v>
       </c>
       <c r="G13">
-        <v>16.30194179501266</v>
+        <v>11.77618746608658</v>
       </c>
       <c r="H13">
-        <v>-0.3162302847897586</v>
+        <v>-0.2288589518366477</v>
       </c>
       <c r="I13">
-        <v>0.83978518420597</v>
+        <v>0.8592237844598907</v>
       </c>
       <c r="J13">
-        <v>0.4584170776515667</v>
+        <v>0.5335169776962454</v>
       </c>
       <c r="K13">
-        <v>0.6060507266209332</v>
+        <v>0.63394175652331</v>
       </c>
     </row>
     <row r="14">
@@ -926,25 +926,25 @@
         <v>5</v>
       </c>
       <c r="E14">
-        <v>0.1475707706689155</v>
+        <v>0.1282826116788999</v>
       </c>
       <c r="F14">
-        <v>0.02824323664088075</v>
+        <v>0.02331397681915248</v>
       </c>
       <c r="G14">
-        <v>0.6269940595996286</v>
+        <v>0.5255336684444168</v>
       </c>
       <c r="H14">
-        <v>-0.01873061043946446</v>
+        <v>-0.01571896525981276</v>
       </c>
       <c r="I14">
-        <v>0.9798184594047777</v>
+        <v>0.9862191523888855</v>
       </c>
       <c r="J14">
-        <v>0.9236747173679887</v>
+        <v>0.9469721082430758</v>
       </c>
       <c r="K14">
-        <v>0.9249043392791494</v>
+        <v>0.9477682981782146</v>
       </c>
     </row>
     <row r="15">
@@ -967,25 +967,25 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <v>0.1853455057126816</v>
+        <v>0.1854237224963548</v>
       </c>
       <c r="F15">
-        <v>0.04786173857393463</v>
+        <v>0.04713375850113642</v>
       </c>
       <c r="G15">
-        <v>1.214347984806394</v>
+        <v>1.001296417951039</v>
       </c>
       <c r="H15">
-        <v>-0.03627702478693588</v>
+        <v>-0.02994925835129821</v>
       </c>
       <c r="I15">
-        <v>0.9672575894201983</v>
+        <v>0.9700023675051184</v>
       </c>
       <c r="J15">
-        <v>0.8795985132320271</v>
+        <v>0.8892103051690939</v>
       </c>
       <c r="K15">
-        <v>0.8842109566755497</v>
+        <v>0.8921005918356066</v>
       </c>
     </row>
     <row r="16">
@@ -1008,25 +1008,25 @@
         <v>20</v>
       </c>
       <c r="E16">
-        <v>0.2769354091848397</v>
+        <v>0.2626065651168993</v>
       </c>
       <c r="F16">
-        <v>0.1067749146063095</v>
+        <v>0.09350780578339697</v>
       </c>
       <c r="G16">
-        <v>2.388086188057374</v>
+        <v>2.127143742047527</v>
       </c>
       <c r="H16">
-        <v>-0.07134088656745997</v>
+        <v>-0.0636238943222143</v>
       </c>
       <c r="I16">
-        <v>0.9196043847048426</v>
+        <v>0.9354540316014135</v>
       </c>
       <c r="J16">
-        <v>0.7312028203491356</v>
+        <v>0.777781642446197</v>
       </c>
       <c r="K16">
-        <v>0.7490407618241506</v>
+        <v>0.7908255968245903</v>
       </c>
     </row>
     <row r="17">
@@ -1049,25 +1049,25 @@
         <v>40</v>
       </c>
       <c r="E17">
-        <v>0.3680515057446886</v>
+        <v>0.3951294098703838</v>
       </c>
       <c r="F17">
-        <v>0.1891763499107949</v>
+        <v>0.199361938009991</v>
       </c>
       <c r="G17">
-        <v>4.750592491743254</v>
+        <v>5.051942597345183</v>
       </c>
       <c r="H17">
-        <v>-0.1419176082406705</v>
+        <v>-0.1511060374443661</v>
       </c>
       <c r="I17">
-        <v>0.8473366294181485</v>
+        <v>0.8347385769282054</v>
       </c>
       <c r="J17">
-        <v>0.5252281859279113</v>
+        <v>0.4969079127510794</v>
       </c>
       <c r="K17">
-        <v>0.5958177170422687</v>
+        <v>0.5704832749700395</v>
       </c>
     </row>
     <row r="18">
@@ -1090,25 +1090,25 @@
         <v>5</v>
       </c>
       <c r="E18">
-        <v>0.09627112839734982</v>
+        <v>0.1221380329802444</v>
       </c>
       <c r="F18">
-        <v>0.01650571314261481</v>
+        <v>0.02187045800782594</v>
       </c>
       <c r="G18">
-        <v>0.0698305897229215</v>
+        <v>0.01882188585003358</v>
       </c>
       <c r="H18">
-        <v>0.002086095638120281</v>
+        <v>-0.0005629716753953907</v>
       </c>
       <c r="I18">
-        <v>0.9916771033111469</v>
+        <v>0.9875334151433026</v>
       </c>
       <c r="J18">
-        <v>0.9675167215501373</v>
+        <v>0.9519303878654223</v>
       </c>
       <c r="K18">
-        <v>0.9675319738789933</v>
+        <v>0.9519314091384667</v>
       </c>
     </row>
     <row r="19">
@@ -1131,25 +1131,25 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <v>0.181771486776869</v>
+        <v>0.1755159288102985</v>
       </c>
       <c r="F19">
-        <v>0.05023031796782555</v>
+        <v>0.0450456767318077</v>
       </c>
       <c r="G19">
-        <v>0.09129489183967666</v>
+        <v>0.06897052873495001</v>
       </c>
       <c r="H19">
-        <v>-0.002727313007166232</v>
+        <v>-0.002062941748993312</v>
       </c>
       <c r="I19">
-        <v>0.968305351662022</v>
+        <v>0.973192132977132</v>
       </c>
       <c r="J19">
-        <v>0.8841971495674434</v>
+        <v>0.9007336968531102</v>
       </c>
       <c r="K19">
-        <v>0.8842232193673591</v>
+        <v>0.9007474101761161</v>
       </c>
     </row>
     <row r="20">
@@ -1172,25 +1172,25 @@
         <v>20</v>
       </c>
       <c r="E20">
-        <v>0.2426126705710935</v>
+        <v>0.2487180774885371</v>
       </c>
       <c r="F20">
-        <v>0.08737892961283765</v>
+        <v>0.08989904407627372</v>
       </c>
       <c r="G20">
-        <v>0.1339244207222853</v>
+        <v>0.04203717288874267</v>
       </c>
       <c r="H20">
-        <v>-0.004000813268441298</v>
+        <v>0.001257352097373332</v>
       </c>
       <c r="I20">
-        <v>0.9390349651987561</v>
+        <v>0.9414194850983194</v>
       </c>
       <c r="J20">
-        <v>0.7937021569373137</v>
+        <v>0.8006650373173626</v>
       </c>
       <c r="K20">
-        <v>0.7937582571224158</v>
+        <v>0.8006701315948495</v>
       </c>
     </row>
     <row r="21">
@@ -1213,25 +1213,25 @@
         <v>40</v>
       </c>
       <c r="E21">
-        <v>0.3296935409754427</v>
+        <v>0.3493049891969582</v>
       </c>
       <c r="F21">
-        <v>0.1705003013623821</v>
+        <v>0.1783333631414632</v>
       </c>
       <c r="G21">
-        <v>1.50933453492303</v>
+        <v>0.05672445803967791</v>
       </c>
       <c r="H21">
-        <v>0.04508935413921789</v>
+        <v>-0.0016966558735365</v>
       </c>
       <c r="I21">
-        <v>0.8707265187565614</v>
+        <v>0.8607018598245459</v>
       </c>
       <c r="J21">
-        <v>0.6190319030979793</v>
+        <v>0.6068318286357915</v>
       </c>
       <c r="K21">
-        <v>0.6261574099085919</v>
+        <v>0.6068411045410677</v>
       </c>
     </row>
     <row r="22">
@@ -1254,25 +1254,25 @@
         <v>5</v>
       </c>
       <c r="E22">
-        <v>0.1334125503621213</v>
+        <v>0.1294871590151127</v>
       </c>
       <c r="F22">
-        <v>0.02557939388499698</v>
+        <v>0.02333603148897975</v>
       </c>
       <c r="G22">
-        <v>0.6136416156001805</v>
+        <v>0.5594626062284366</v>
       </c>
       <c r="H22">
-        <v>-0.01833172400164378</v>
+        <v>-0.01673379613812357</v>
       </c>
       <c r="I22">
-        <v>0.9836824947260077</v>
+        <v>0.9859510106246359</v>
       </c>
       <c r="J22">
-        <v>0.9376177401693087</v>
+        <v>0.9459715908755906</v>
       </c>
       <c r="K22">
-        <v>0.9387955477641925</v>
+        <v>0.9468739049314069</v>
       </c>
     </row>
     <row r="23">
@@ -1295,25 +1295,25 @@
         <v>10</v>
       </c>
       <c r="E23">
-        <v>0.1823155423685806</v>
+        <v>0.1825755512972048</v>
       </c>
       <c r="F23">
-        <v>0.04677270486575666</v>
+        <v>0.04649145484630868</v>
       </c>
       <c r="G23">
-        <v>1.259060721192102</v>
+        <v>1.105726015480153</v>
       </c>
       <c r="H23">
-        <v>-0.03761275809110459</v>
+        <v>-0.03307279793443338</v>
       </c>
       <c r="I23">
-        <v>0.9684386137408849</v>
+        <v>0.9710307711694485</v>
       </c>
       <c r="J23">
-        <v>0.8835028990438965</v>
+        <v>0.8925876999439615</v>
       </c>
       <c r="K23">
-        <v>0.8884612594631727</v>
+        <v>0.8961123065422846</v>
       </c>
     </row>
     <row r="24">
@@ -1336,25 +1336,25 @@
         <v>20</v>
       </c>
       <c r="E24">
-        <v>0.2401795482448199</v>
+        <v>0.2663383968565355</v>
       </c>
       <c r="F24">
-        <v>0.08639366861902853</v>
+        <v>0.09543493023529215</v>
       </c>
       <c r="G24">
-        <v>2.166054113556416</v>
+        <v>2.439108068645621</v>
       </c>
       <c r="H24">
-        <v>-0.06470797477368759</v>
+        <v>-0.07295489765566668</v>
       </c>
       <c r="I24">
-        <v>0.9424438351737155</v>
+        <v>0.9337840851572148</v>
       </c>
       <c r="J24">
-        <v>0.79781926187243</v>
+        <v>0.7714209951520811</v>
       </c>
       <c r="K24">
-        <v>0.8124944387869377</v>
+        <v>0.7885715304664422</v>
       </c>
     </row>
     <row r="25">
@@ -1377,25 +1377,25 @@
         <v>40</v>
       </c>
       <c r="E25">
-        <v>0.3900148873318768</v>
+        <v>0.409150627249522</v>
       </c>
       <c r="F25">
-        <v>0.2024396815512325</v>
+        <v>0.2076560953838874</v>
       </c>
       <c r="G25">
-        <v>5.787952748800723</v>
+        <v>5.813976309088061</v>
       </c>
       <c r="H25">
-        <v>-0.1729073609549683</v>
+        <v>-0.1738988329604909</v>
       </c>
       <c r="I25">
-        <v>0.8307124016163758</v>
+        <v>0.8250723763962009</v>
       </c>
       <c r="J25">
-        <v>0.4668737089069579</v>
+        <v>0.4605698486428372</v>
       </c>
       <c r="K25">
-        <v>0.5716576418410352</v>
+        <v>0.5580154207913334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>